<commit_message>
update harvesting templates, info texts
</commit_message>
<xml_diff>
--- a/ckanext/lhm/schemas/template_gdp_v1.2.4.xlsx
+++ b/ckanext/lhm/schemas/template_gdp_v1.2.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mb\dev\ckan-docker\ckan\new_oracle_data_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\mb\p2\ckan-tools\gdp_harvesting\schema_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12622FCB-1A50-4B4F-9F8C-2CEB3E98D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BEA707-671B-477E-88EB-5FF86CD8CC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="504" windowWidth="23040" windowHeight="11460" tabRatio="871" xr2:uid="{EFAD0BDA-2C19-4F99-80E8-84599936D919}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{EFAD0BDA-2C19-4F99-80E8-84599936D919}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadaten" sheetId="1" r:id="rId1"/>
@@ -1972,12 +1972,12 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Schlagworte sind i.d.R. Substantive zur inhaltlichen Beschreibung des Datensatzes. Es können mehrere Schlagworte vergeben werden." sqref="B5" xr:uid="{623C178E-EC83-43E9-958F-0440F931AA20}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Hier können ergänzende Informationen zur Lagegenauigkeit ergänzt werden, beispielsweise ein geeigneter Maßstab (z.B. 1:500), die Größe eines Pixels (z.B. 20cm) oder die Spanne der Abweichung bei der Lage (z.B. +/- 10m)." sqref="B9" xr:uid="{970220F6-FBF5-4CF5-BE13-F3DFE3BCB688}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Angabe des fachlich zuständigen Referats und der ersten, das Referat untergliedernden Organisationseinheit (z.B. Amt, Hauptabteilung, Geschäftsbereich)" sqref="B10" xr:uid="{09939F82-660A-44C0-8D41-AB87CD53810A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Angabe der Stelle, die fachliche und organisatorische Kenntnis zum Datensatz hat" sqref="B11" xr:uid="{BE1FC14A-141B-48FB-BA17-F9E0540C34BB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Angabe der Organisationseinheit, die fachliche und organisatorische Kenntnis zum Datensatz hat" sqref="B11" xr:uid="{BE1FC14A-141B-48FB-BA17-F9E0540C34BB}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Zusätzliche Hinweise zur Nutzung können unter 'Hinweise' mit Stichwort und Erklärung eingefügt werden. Diese müssen auch für Laien verständlich sein. Hinweise können z.B. zu vertraglichen Bedingungen oder Besonderheiten des Datensatzes erfolgen._x000a__x000a_" sqref="B28" xr:uid="{41DA2449-4EB8-42B0-8B24-A586BE48D043}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Um externe Datenurheber handelt es sich, wenn die Daten nicht von der Landeshautpststadt München stammen (z.B. LDBV)." sqref="B13" xr:uid="{6FD9F116-7FAD-43B8-974A-91F50455A327}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zugriffsuser" prompt="Ist der Zugriff auf bestimmte Zugriffsuser zu beschränken, sind hier die entsprechenden User anzugeben (Komma als Trennzeichen)" sqref="B18" xr:uid="{5BFD9ECE-5759-4364-8421-D1A1E51E2D29}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Eingeschränkter Zugriff" prompt="Ist der Zugriff auf bestimmte Gruppen/Organisationseinheiten im GeoInfoWeb zu beschränken, sind hier die entsprechenden Gruppen/Organisationseinheiten anzugeben (Komma als Trennzeichen)" sqref="B20" xr:uid="{E9F37E1E-B0FC-4703-9265-EF66076FF35D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name des Datenbankschemas" prompt="(beim Geodatenpool z.B. BAUT, PLAN, RKU)." sqref="B3" xr:uid="{C8676A5A-F5FC-4B9E-975C-CB6983604CAE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name des Datenbankschemas" prompt="(z.B. BAU, PLAN, RKU im Geodatenpool)" sqref="B3" xr:uid="{C8676A5A-F5FC-4B9E-975C-CB6983604CAE}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Auswahl legt fest, ob Daten für Backend und Präsentation, externe Auftragnehmer (mit Vertrag) oder sonstige Dritte (mit Bedingungen) nutzbar sind. Einschränkungen können bestimmte Inhalte oder Attribute betreffen. Ausführliche Hinweise zum Feld s.u." sqref="B22" xr:uid="{3865BC3F-EC1E-43CB-A54F-659A2F5AB813}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mit dem Updatezyklus kann angegeben werden, ob und wie regelmäßig die Daten in der Datenbank aktualisiert werden." sqref="B14" xr:uid="{BD09D3BE-047F-41E0-9A7E-A7A85A3369A6}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Die Bewertung der Archivwürdigkeit erfolgt durch das Stadtarchiv" sqref="B15" xr:uid="{8A048881-B550-43EE-805E-C2EA2A69558E}"/>

</xml_diff>

<commit_message>
remove dropdowns in export templates, sheets dv, dd
</commit_message>
<xml_diff>
--- a/ckanext/lhm/schemas/template_gdp_v1.2.4.xlsx
+++ b/ckanext/lhm/schemas/template_gdp_v1.2.4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\mb\p2\ckan-tools\gdp_harvesting\schema_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\mb\p2\ckanext-lhm\ckanext\lhm\schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BEA707-671B-477E-88EB-5FF86CD8CC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DFC6E1-B5E6-4B14-AF2B-82F5F5D8EBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{EFAD0BDA-2C19-4F99-80E8-84599936D919}"/>
   </bookViews>
@@ -1037,14 +1037,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1815,7 +1815,7 @@
       <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="29" t="s">
         <v>105</v>
       </c>
       <c r="B28" s="19"/>
@@ -1906,60 +1906,60 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+      <c r="A45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2051,18 +2051,6 @@
   <headerFooter>
     <oddHeader>&amp;A</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D6A376D-F7FC-4BCE-B041-38F3CB82F992}">
-          <x14:formula1>
-            <xm:f>Wertelisten!$O$2:$O$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2143,18 +2131,6 @@
   <headerFooter>
     <oddHeader>&amp;A</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5649EDE8-8F38-4B5C-ADEA-718A5042BAE4}">
-          <x14:formula1>
-            <xm:f>Wertelisten!$R$2:$R$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>